<commit_message>
Beta2: add output list with missing key-mapping
</commit_message>
<xml_diff>
--- a/conversion_remapping.xlsx
+++ b/conversion_remapping.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\Remapping Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAB81E8-CA16-4100-856F-513A9D8AEBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{E55BB45E-B1F2-4434-8CA3-7712472E0AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" windowHeight="12360" windowWidth="24285" xWindow="76920" xr2:uid="{1E709FDD-82E7-4D18-BDFE-969612B1B9EE}" yWindow="8340"/>
+    <workbookView xWindow="22065" yWindow="7725" windowWidth="42885" windowHeight="12360" xr2:uid="{1E709FDD-82E7-4D18-BDFE-969612B1B9EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Explanation" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Settings" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="97">
   <si>
     <t>New_Variable</t>
   </si>
@@ -288,69 +289,27 @@
     <t>1</t>
   </si>
   <si>
-    <t>Normal,Unit,Check2Option,Option2Check,ID</t>
-  </si>
-  <si>
-    <t>Normal,Unit,Check2Option,Option2Check,ID</t>
-  </si>
-  <si>
-    <t>temp_A</t>
-  </si>
-  <si>
-    <t>temp_B</t>
-  </si>
-  <si>
     <t>A_set</t>
   </si>
   <si>
     <t>B_set</t>
   </si>
   <si>
-    <t>tem_B</t>
-  </si>
-  <si>
     <t>Swap</t>
   </si>
   <si>
-    <t>Normal,Unit,Check2Option,Option2Check,ID</t>
-  </si>
-  <si>
-    <t>Normal,Unit,Check2Option,Option2Check,ID</t>
-  </si>
-  <si>
-    <t>Swam</t>
-  </si>
-  <si>
     <t>Swamps the sets, A_set -&gt; B_set &amp; B_set to A_set</t>
   </si>
   <si>
-    <t>Don forget to add this one, other wise it would be in the output</t>
-  </si>
-  <si>
     <t>**Don't forget to add this line, otherwise B_set won't appear in the output</t>
   </si>
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>D-M-Y</t>
-  </si>
-  <si>
-    <t>%D-%M-%Y</t>
-  </si>
-  <si>
-    <t>%D/%M/%Y</t>
-  </si>
-  <si>
-    <t>%D/%m/%Y</t>
-  </si>
-  <si>
     <t>%d/%m/%Y</t>
   </si>
   <si>
-    <t>Converts the format in column D into ISO 8601 (%Y-%m-%d)</t>
-  </si>
-  <si>
     <t>Converts the format in column D into ISO 8601 (%Y-%m-%d), errors will be coded in the output to: "ERR: original value"</t>
   </si>
   <si>
@@ -360,19 +319,10 @@
     <t>End_Date</t>
   </si>
   <si>
-    <t>%Y-%m-%d</t>
-  </si>
-  <si>
     <t>A_dur</t>
   </si>
   <si>
     <t>Duration</t>
-  </si>
-  <si>
-    <t>{"Start_Date": "End_Date"}</t>
-  </si>
-  <si>
-    <t>End_date</t>
   </si>
   <si>
     <t>%d-%m-%Y</t>
@@ -384,79 +334,84 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" count="8" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
-    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
-    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF006100"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF9C5700"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="8"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b/>
-      <color rgb="FF000000"/>
-      <sz val="16"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -485,74 +440,74 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC00"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF8EAADB"/>
       </top>
       <bottom style="thin">
         <color rgb="FF8EAADB"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-  </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
@@ -633,8 +588,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9AE4542F-9F68-485E-BBE8-B9FEA9E3DC09}" name="Table15" displayName="Table15" ref="A2:D15" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A2:D15" xr:uid="{383FDB88-F083-4CDF-B03D-AFE7141D47C4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9AE4542F-9F68-485E-BBE8-B9FEA9E3DC09}" name="Table15" displayName="Table15" ref="A2:D20" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A2:D20" xr:uid="{383FDB88-F083-4CDF-B03D-AFE7141D47C4}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{F3CBDC26-DCC0-4BFD-8D06-40CD89F11564}" name="New_Variable"/>
     <tableColumn id="2" xr3:uid="{B0CC8640-035B-44C3-BEBB-26EF34860A55}" name="TypeOfConversion"/>
@@ -646,19 +601,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0210BAFE-84A8-49BE-B784-1E712D070C04}" name="Table36" displayName="Table36" ref="A19:B25" totalsRowShown="0">
-  <autoFilter ref="A19:B25" xr:uid="{0210BAFE-84A8-49BE-B784-1E712D070C04}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CC970CBD-E349-4DB1-968F-53A94B087448}" name="Item"/>
-    <tableColumn id="2" xr3:uid="{B80B0D2B-509E-4C15-A8D1-E0AD6D328D62}" name="Variable"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{383FDB88-F083-4CDF-B03D-AFE7141D47C4}" name="Table1" displayName="Table1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:D14" xr:uid="{383FDB88-F083-4CDF-B03D-AFE7141D47C4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{383FDB88-F083-4CDF-B03D-AFE7141D47C4}" name="Table1" displayName="Table1" ref="A1:D19" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:D19" xr:uid="{383FDB88-F083-4CDF-B03D-AFE7141D47C4}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{E142AF83-5691-4FFC-9325-BE0C7B6FEAEA}" name="New_Variable" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{E2732F87-DBC8-4585-9AD9-9E2C28FCE04F}" name="TypeOfConversion" dataDxfId="6"/>
@@ -669,7 +613,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60E7149A-D671-4822-9274-9F55ED5DFB04}" name="Table2" displayName="Table2" ref="A1:B5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B5" xr:uid="{60E7149A-D671-4822-9274-9F55ED5DFB04}"/>
   <tableColumns count="2">
@@ -680,7 +624,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{876848A8-AE83-4E67-8B2D-2B10383227A5}" name="Table3" displayName="Table3" ref="A1:B7" totalsRowShown="0">
   <autoFilter ref="A1:B7" xr:uid="{876848A8-AE83-4E67-8B2D-2B10383227A5}"/>
   <tableColumns count="2">
@@ -987,23 +931,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB16E3F3-6009-44A7-8F83-4CBF6605F01E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB16E3F3-6009-44A7-8F83-4CBF6605F01E}">
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView zoomScale="160" workbookViewId="0" zoomScaleNormal="160">
-      <selection pane="topLeft" activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" customWidth="1"/>
     <col min="7" max="7" width="24.140625" customWidth="1"/>
-    <col min="8" max="8" width="8.26" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="21" r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>52</v>
       </c>
@@ -1191,12 +1136,12 @@
       <c r="D12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1208,12 +1153,12 @@
       <c r="C13" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1228,12 +1173,12 @@
       <c r="D14">
         <v>4</v>
       </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1246,36 +1191,36 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>88</v>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" t="s">
+        <v>84</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>88</v>
+      <c r="C17" t="s">
+        <v>84</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -1285,62 +1230,68 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18">
-      <c r="A18" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>102</v>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
+        <v>89</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>112</v>
+        <v>88</v>
+      </c>
+      <c r="H18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" t="s">
+        <v>95</v>
       </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20">
-      <c r="A20" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>105</v>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" t="s">
+        <v>91</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>94</v>
+      </c>
+      <c r="H20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
       <c r="G22" s="5" t="s">
         <v>49</v>
       </c>
@@ -1351,7 +1302,9 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
       <c r="G23" s="5" t="s">
         <v>50</v>
       </c>
@@ -1362,7 +1315,9 @@
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
       <c r="G24" s="5" t="s">
         <v>51</v>
       </c>
@@ -1373,12 +1328,13 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
     </row>
-    <row ht="21" r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+      <c r="A25" s="12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="11"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1386,7 +1342,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1397,7 +1353,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1408,7 +1364,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1419,7 +1375,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1430,7 +1386,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -1441,7 +1397,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -1452,7 +1408,7 @@
         <v>59</v>
       </c>
     </row>
-    <row ht="21" r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
         <v>61</v>
       </c>
@@ -1510,7 +1466,7 @@
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="7:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G40" s="8" t="s">
         <v>69</v>
       </c>
@@ -1520,7 +1476,7 @@
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
     </row>
-    <row r="41" spans="7:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G41" s="8" t="s">
         <v>70</v>
       </c>
@@ -1532,27 +1488,27 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B20" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Normal,Unit,Check2Option,Option2Check,ID"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="1">
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760AE619-E443-4395-BB8D-172BD6E93BCC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760AE619-E443-4395-BB8D-172BD6E93BCC}">
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView zoomScale="205" workbookViewId="0" tabSelected="1" zoomScaleNormal="205">
-      <selection pane="topLeft" activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A10" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
@@ -1743,74 +1699,76 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" s="0" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="0" t="s">
+      <c r="C17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>105</v>
+      <c r="C18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6 B9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6 B9" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Normal,Unit,Check2Option,Option2Check,ID"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1823,13 +1781,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FACC24-7102-4663-A563-97415C02CCA1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FACC24-7102-4663-A563-97415C02CCA1}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView zoomScale="205" workbookViewId="0" zoomScaleNormal="205">
-      <selection pane="topLeft" activeCell="A2" sqref="A2:B5"/>
+    <sheetView topLeftCell="A4" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" style="3" customWidth="1"/>
@@ -1885,13 +1844,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{647F3D03-9604-45FA-805B-B7EE8B0FC232}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{647F3D03-9604-45FA-805B-B7EE8B0FC232}">
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="175" workbookViewId="0" zoomScaleNormal="175">
-      <selection pane="topLeft" activeCell="B2" sqref="B2:B7"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>

</xml_diff>